<commit_message>
CheckList de Aseguramiento de la Calidad
</commit_message>
<xml_diff>
--- a/Area_de_Proceso-_PPQA/CHKQA/CHKQA_V1.1_2015.xlsx
+++ b/Area_de_Proceso-_PPQA/CHKQA/CHKQA_V1.1_2015.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thefa\Documents\GitHub\UTP-GPS-ALARM\Area_de_Proceso-_PPQA\CHKQA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jleonardo\Documents\GitHub\UTP-GPS-ALARM\Area_de_Proceso-_PPQA\CHKQA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -54,12 +54,12 @@
     <definedName name="TiposCausa" localSheetId="0">[2]Instructivo!$B$38:$B$46</definedName>
     <definedName name="TipoServicio" localSheetId="0">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4399" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4399" uniqueCount="479">
   <si>
     <r>
       <t xml:space="preserve">¿El objeto i de información tiene la sección </t>
@@ -3117,11 +3117,161 @@
   <si>
     <t>Versión Final pendiente de Aprobación</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Documento : Informe de Pruebas Externas                                                              [INPRUEX]_[DD]_[MM]_[2015]        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                      GitHub\UTP-GPS-ALARM\tree\master\Area_de_Proceso-_REQM\Ingeniería\INPRUEX</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Documento : Informe de Pruebas Internas                                                              [INPRUIN]_[DD]_[MM]_[2015]         </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                    GitHub\UTP-GPS-ALARM\tree\master\Area_de_Proceso-_REQM\Ingeniería\INPRUIN</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Documento : Acta de Solicitud de Cambios a Requerimientos                                                               [ASCR]_[DD]_[MM]_[2015]                                                                                                                 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>GitHub\UTP-GPS-ALARM\tree\master\Area_de_Proceso-_REQM\ASCR</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Documento : Acta de Cierre de Proyecto                                                                            [ACCPRO]_[DD]_[MM]_[2015]                                                                                                         </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>GitHub\UTP-GPS-ALARM\tree\master\Area_de_Proceso-_PP-PMC\ACCPRO</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Documento : Acta de Relatorio de Proyecto                                                                              [ACREVPRO]_[DD]_[MM]_[2015]                       </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                GitHub\UTP-GPS-ALARM\tree\master\Area_de_Proceso-_PP-PMC\ACREVPRO</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Documento : Solicitud de Aseguramiento de Calidad                                                         [SOLQA]_[DD]_[MM]_[2015]                                                                                                      </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>GitHub\UTP-GPS-ALARM\tree\master\Area_de_Proceso-_PPQA\SOLQA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Documento : Informe de Avance Quincenal                                             [IAVQUI]_[DD]_[MM]_[2015]                                                                                                          </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>GitHub\UTP-GPS-ALARM\tree\master\Informes\IAVQUI</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Documento : Acta de Aceptación  de Entregables                                               [ACENTRE]_[DD]_[MM]_[2015]                                                                                                       </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>GitHub\UTP-GPS-ALARM\tree\master\Actas\ACENTRE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Documento : Acta de reunión Interna                                                   [ARINT]_[DD]_[MM]_[2015]                                                                                                       </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>GitHub\UTP-GPS-ALARM\tree\master\Actas\ARINT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Documento : Acta de reunión Externa                                                 [AREXT]_[DD]_[MM]_[2015]                                                                                                       </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>GitHub\UTP-GPS-ALARM\tree\master\Actas\AREXT</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_([$€-2]\ * #,##0.00_);_([$€-2]\ * \(#,##0.00\);_([$€-2]\ * &quot;-&quot;??_)"/>
   </numFmts>
@@ -5788,24 +5938,6 @@
     <xf numFmtId="0" fontId="1" fillId="29" borderId="0" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="10" xfId="39" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="36" xfId="39" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="12" xfId="39" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5842,6 +5974,15 @@
     <xf numFmtId="0" fontId="3" fillId="29" borderId="0" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="10" xfId="39" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="36" xfId="39" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="12" xfId="39" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5849,6 +5990,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -6533,7 +6683,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -6670,7 +6820,7 @@
                     <a:cs typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="es-PE"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="ctr"/>
@@ -6681,7 +6831,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -6708,7 +6858,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-4A15-4F9A-9387-0E32CA9DDB24}"/>
             </c:ext>
@@ -6788,7 +6938,7 @@
                       <a:cs typeface="Arial"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-PE"/>
                 </a:p>
               </c:txPr>
               <c:dLblPos val="outEnd"/>
@@ -6798,11 +6948,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-4A15-4F9A-9387-0E32CA9DDB24}"/>
                 </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -6827,7 +6977,7 @@
                     <a:cs typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="es-PE"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -6837,7 +6987,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -6855,7 +7005,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-4A15-4F9A-9387-0E32CA9DDB24}"/>
             </c:ext>
@@ -6935,7 +7085,7 @@
                       <a:cs typeface="Arial"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-PE"/>
                 </a:p>
               </c:txPr>
               <c:dLblPos val="outEnd"/>
@@ -6945,11 +7095,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-4A15-4F9A-9387-0E32CA9DDB24}"/>
                 </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -6974,7 +7124,7 @@
                     <a:cs typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="es-PE"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -6984,7 +7134,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -7002,7 +7152,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-4A15-4F9A-9387-0E32CA9DDB24}"/>
             </c:ext>
@@ -7017,11 +7167,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="281559304"/>
-        <c:axId val="281558128"/>
+        <c:axId val="394149072"/>
+        <c:axId val="394002040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="281559304"/>
+        <c:axId val="394149072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7053,10 +7203,10 @@
                 <a:cs typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="281558128"/>
+        <c:crossAx val="394002040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -7066,7 +7216,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="281558128"/>
+        <c:axId val="394002040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7108,10 +7258,10 @@
                 <a:cs typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="281559304"/>
+        <c:crossAx val="394149072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7165,7 +7315,7 @@
               <a:cs typeface="Arial"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-PE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -7198,7 +7348,7 @@
           <a:cs typeface="Arial"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-PE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -12201,22 +12351,22 @@
       <c r="A18" s="28"/>
     </row>
     <row r="19" spans="1:5" s="16" customFormat="1" ht="16.5" customHeight="1">
-      <c r="B19" s="481" t="s">
+      <c r="B19" s="478" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="482"/>
-      <c r="D19" s="482"/>
-      <c r="E19" s="483"/>
+      <c r="C19" s="479"/>
+      <c r="D19" s="479"/>
+      <c r="E19" s="480"/>
     </row>
     <row r="20" spans="1:5" s="16" customFormat="1" ht="13.5" customHeight="1">
       <c r="B20" s="446" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="463" t="s">
+      <c r="C20" s="481" t="s">
         <v>134</v>
       </c>
-      <c r="D20" s="464"/>
-      <c r="E20" s="465"/>
+      <c r="D20" s="482"/>
+      <c r="E20" s="483"/>
     </row>
     <row r="21" spans="1:5" s="16" customFormat="1" ht="12.75" customHeight="1">
       <c r="B21" s="33" t="s">
@@ -12269,249 +12419,249 @@
       <c r="B26" s="23"/>
     </row>
     <row r="27" spans="1:5" s="16" customFormat="1" ht="16.5" customHeight="1">
-      <c r="B27" s="481" t="s">
+      <c r="B27" s="478" t="s">
         <v>456</v>
       </c>
-      <c r="C27" s="482"/>
-      <c r="D27" s="482"/>
-      <c r="E27" s="483"/>
+      <c r="C27" s="479"/>
+      <c r="D27" s="479"/>
+      <c r="E27" s="480"/>
     </row>
     <row r="28" spans="1:5" s="16" customFormat="1" ht="13.5" customHeight="1">
       <c r="B28" s="446" t="s">
         <v>71</v>
       </c>
-      <c r="C28" s="463" t="s">
+      <c r="C28" s="481" t="s">
         <v>134</v>
       </c>
-      <c r="D28" s="464"/>
-      <c r="E28" s="465"/>
+      <c r="D28" s="482"/>
+      <c r="E28" s="483"/>
     </row>
     <row r="29" spans="1:5" ht="15.95" customHeight="1">
       <c r="A29" s="28"/>
-      <c r="B29" s="474" t="s">
+      <c r="B29" s="468" t="s">
         <v>49</v>
       </c>
-      <c r="C29" s="475"/>
-      <c r="D29" s="475"/>
-      <c r="E29" s="476"/>
+      <c r="C29" s="469"/>
+      <c r="D29" s="469"/>
+      <c r="E29" s="470"/>
     </row>
     <row r="30" spans="1:5" ht="15.95" customHeight="1">
       <c r="A30" s="28"/>
       <c r="B30" s="46" t="s">
         <v>270</v>
       </c>
-      <c r="C30" s="466" t="s">
+      <c r="C30" s="475" t="s">
         <v>271</v>
       </c>
-      <c r="D30" s="467"/>
-      <c r="E30" s="468"/>
+      <c r="D30" s="476"/>
+      <c r="E30" s="477"/>
     </row>
     <row r="31" spans="1:5" ht="15.95" customHeight="1">
       <c r="A31" s="28"/>
       <c r="B31" s="46" t="s">
         <v>267</v>
       </c>
-      <c r="C31" s="466" t="s">
+      <c r="C31" s="475" t="s">
         <v>160</v>
       </c>
-      <c r="D31" s="467"/>
-      <c r="E31" s="468"/>
+      <c r="D31" s="476"/>
+      <c r="E31" s="477"/>
     </row>
     <row r="32" spans="1:5" ht="15.95" customHeight="1">
       <c r="A32" s="28"/>
       <c r="B32" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="C32" s="466" t="s">
+      <c r="C32" s="475" t="s">
         <v>75</v>
       </c>
-      <c r="D32" s="467"/>
-      <c r="E32" s="468"/>
+      <c r="D32" s="476"/>
+      <c r="E32" s="477"/>
     </row>
     <row r="33" spans="1:5" ht="15.95" customHeight="1">
       <c r="A33" s="28"/>
       <c r="B33" s="46" t="s">
         <v>268</v>
       </c>
-      <c r="C33" s="466" t="s">
+      <c r="C33" s="475" t="s">
         <v>269</v>
       </c>
-      <c r="D33" s="467"/>
-      <c r="E33" s="468"/>
+      <c r="D33" s="476"/>
+      <c r="E33" s="477"/>
     </row>
     <row r="34" spans="1:5" ht="15.95" customHeight="1">
       <c r="A34" s="28"/>
       <c r="B34" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="C34" s="466" t="s">
+      <c r="C34" s="475" t="s">
         <v>77</v>
       </c>
-      <c r="D34" s="467"/>
-      <c r="E34" s="468"/>
+      <c r="D34" s="476"/>
+      <c r="E34" s="477"/>
     </row>
     <row r="35" spans="1:5" ht="15.95" customHeight="1">
       <c r="A35" s="28"/>
       <c r="B35" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="C35" s="466" t="s">
+      <c r="C35" s="475" t="s">
         <v>73</v>
       </c>
-      <c r="D35" s="467"/>
-      <c r="E35" s="468"/>
+      <c r="D35" s="476"/>
+      <c r="E35" s="477"/>
     </row>
     <row r="36" spans="1:5" ht="27.75" customHeight="1">
       <c r="A36" s="28"/>
       <c r="B36" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="C36" s="466" t="s">
+      <c r="C36" s="475" t="s">
         <v>79</v>
       </c>
-      <c r="D36" s="467"/>
-      <c r="E36" s="468"/>
+      <c r="D36" s="476"/>
+      <c r="E36" s="477"/>
     </row>
     <row r="37" spans="1:5" ht="15.95" customHeight="1">
       <c r="A37" s="28"/>
-      <c r="B37" s="474" t="s">
+      <c r="B37" s="468" t="s">
         <v>50</v>
       </c>
-      <c r="C37" s="475"/>
-      <c r="D37" s="475"/>
-      <c r="E37" s="476"/>
+      <c r="C37" s="469"/>
+      <c r="D37" s="469"/>
+      <c r="E37" s="470"/>
     </row>
     <row r="38" spans="1:5" ht="15.95" customHeight="1">
       <c r="A38" s="28"/>
       <c r="B38" s="46" t="s">
         <v>275</v>
       </c>
-      <c r="C38" s="477" t="s">
+      <c r="C38" s="471" t="s">
         <v>316</v>
       </c>
-      <c r="D38" s="478"/>
-      <c r="E38" s="479"/>
+      <c r="D38" s="472"/>
+      <c r="E38" s="473"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="28"/>
       <c r="B39" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="C39" s="466" t="s">
+      <c r="C39" s="475" t="s">
         <v>317</v>
       </c>
-      <c r="D39" s="467"/>
-      <c r="E39" s="468"/>
+      <c r="D39" s="476"/>
+      <c r="E39" s="477"/>
     </row>
     <row r="40" spans="1:5" ht="15.95" customHeight="1">
       <c r="A40" s="28"/>
       <c r="B40" s="46" t="s">
         <v>134</v>
       </c>
-      <c r="C40" s="466" t="s">
+      <c r="C40" s="475" t="s">
         <v>318</v>
       </c>
-      <c r="D40" s="467"/>
-      <c r="E40" s="468"/>
+      <c r="D40" s="476"/>
+      <c r="E40" s="477"/>
     </row>
     <row r="41" spans="1:5" ht="15.95" customHeight="1">
       <c r="A41" s="28"/>
       <c r="B41" s="46" t="s">
         <v>126</v>
       </c>
-      <c r="C41" s="466" t="s">
+      <c r="C41" s="475" t="s">
         <v>86</v>
       </c>
-      <c r="D41" s="467"/>
-      <c r="E41" s="468"/>
+      <c r="D41" s="476"/>
+      <c r="E41" s="477"/>
     </row>
     <row r="42" spans="1:5" ht="15.95" customHeight="1">
       <c r="A42" s="28"/>
       <c r="B42" s="46" t="s">
         <v>138</v>
       </c>
-      <c r="C42" s="466" t="s">
+      <c r="C42" s="475" t="s">
         <v>83</v>
       </c>
-      <c r="D42" s="467"/>
-      <c r="E42" s="468"/>
+      <c r="D42" s="476"/>
+      <c r="E42" s="477"/>
     </row>
     <row r="43" spans="1:5" ht="15.95" customHeight="1">
       <c r="A43" s="28"/>
       <c r="B43" s="46" t="s">
         <v>137</v>
       </c>
-      <c r="C43" s="466" t="s">
+      <c r="C43" s="475" t="s">
         <v>80</v>
       </c>
-      <c r="D43" s="467"/>
-      <c r="E43" s="468"/>
+      <c r="D43" s="476"/>
+      <c r="E43" s="477"/>
     </row>
     <row r="44" spans="1:5" ht="15.95" customHeight="1">
       <c r="A44" s="28"/>
       <c r="B44" s="46" t="s">
         <v>126</v>
       </c>
-      <c r="C44" s="466" t="s">
+      <c r="C44" s="475" t="s">
         <v>86</v>
       </c>
-      <c r="D44" s="467"/>
-      <c r="E44" s="468"/>
+      <c r="D44" s="476"/>
+      <c r="E44" s="477"/>
     </row>
     <row r="45" spans="1:5" ht="15.95" customHeight="1">
       <c r="A45" s="28"/>
       <c r="B45" s="46" t="s">
         <v>139</v>
       </c>
-      <c r="C45" s="466" t="s">
+      <c r="C45" s="475" t="s">
         <v>84</v>
       </c>
-      <c r="D45" s="467"/>
-      <c r="E45" s="468"/>
+      <c r="D45" s="476"/>
+      <c r="E45" s="477"/>
     </row>
     <row r="46" spans="1:5" ht="15.95" customHeight="1">
       <c r="A46" s="28"/>
       <c r="B46" s="46" t="s">
         <v>137</v>
       </c>
-      <c r="C46" s="466" t="s">
+      <c r="C46" s="475" t="s">
         <v>81</v>
       </c>
-      <c r="D46" s="467"/>
-      <c r="E46" s="468"/>
+      <c r="D46" s="476"/>
+      <c r="E46" s="477"/>
     </row>
     <row r="47" spans="1:5" ht="15.95" customHeight="1">
       <c r="A47" s="28"/>
       <c r="B47" s="46" t="s">
         <v>126</v>
       </c>
-      <c r="C47" s="466" t="s">
+      <c r="C47" s="475" t="s">
         <v>86</v>
       </c>
-      <c r="D47" s="467"/>
-      <c r="E47" s="468"/>
+      <c r="D47" s="476"/>
+      <c r="E47" s="477"/>
     </row>
     <row r="48" spans="1:5" ht="15.95" customHeight="1">
       <c r="A48" s="28"/>
       <c r="B48" s="46" t="s">
         <v>140</v>
       </c>
-      <c r="C48" s="466" t="s">
+      <c r="C48" s="475" t="s">
         <v>85</v>
       </c>
-      <c r="D48" s="467"/>
-      <c r="E48" s="468"/>
+      <c r="D48" s="476"/>
+      <c r="E48" s="477"/>
     </row>
     <row r="49" spans="1:5" ht="15.95" customHeight="1">
       <c r="A49" s="28"/>
       <c r="B49" s="46" t="s">
         <v>137</v>
       </c>
-      <c r="C49" s="466" t="s">
+      <c r="C49" s="475" t="s">
         <v>82</v>
       </c>
-      <c r="D49" s="467"/>
-      <c r="E49" s="468"/>
+      <c r="D49" s="476"/>
+      <c r="E49" s="477"/>
     </row>
     <row r="50" spans="1:5" s="16" customFormat="1" ht="13.5" customHeight="1">
       <c r="B50" s="370"/>
@@ -12527,249 +12677,249 @@
       <c r="E51" s="308"/>
     </row>
     <row r="52" spans="1:5" s="16" customFormat="1" ht="16.5" customHeight="1">
-      <c r="B52" s="481" t="s">
+      <c r="B52" s="478" t="s">
         <v>457</v>
       </c>
-      <c r="C52" s="482"/>
-      <c r="D52" s="482"/>
-      <c r="E52" s="483"/>
+      <c r="C52" s="479"/>
+      <c r="D52" s="479"/>
+      <c r="E52" s="480"/>
     </row>
     <row r="53" spans="1:5" s="16" customFormat="1" ht="13.5" customHeight="1">
       <c r="B53" s="446" t="s">
         <v>71</v>
       </c>
-      <c r="C53" s="463" t="s">
+      <c r="C53" s="481" t="s">
         <v>134</v>
       </c>
-      <c r="D53" s="464"/>
-      <c r="E53" s="465"/>
+      <c r="D53" s="482"/>
+      <c r="E53" s="483"/>
     </row>
     <row r="54" spans="1:5" ht="15.95" customHeight="1">
       <c r="A54" s="28"/>
-      <c r="B54" s="474" t="s">
+      <c r="B54" s="468" t="s">
         <v>49</v>
       </c>
-      <c r="C54" s="475"/>
-      <c r="D54" s="475"/>
-      <c r="E54" s="476"/>
+      <c r="C54" s="469"/>
+      <c r="D54" s="469"/>
+      <c r="E54" s="470"/>
     </row>
     <row r="55" spans="1:5" ht="15.95" customHeight="1">
       <c r="A55" s="28"/>
       <c r="B55" s="46" t="s">
         <v>270</v>
       </c>
-      <c r="C55" s="466" t="s">
+      <c r="C55" s="475" t="s">
         <v>271</v>
       </c>
-      <c r="D55" s="467"/>
-      <c r="E55" s="468"/>
+      <c r="D55" s="476"/>
+      <c r="E55" s="477"/>
     </row>
     <row r="56" spans="1:5" ht="15.95" customHeight="1">
       <c r="A56" s="28"/>
       <c r="B56" s="46" t="s">
         <v>267</v>
       </c>
-      <c r="C56" s="466" t="s">
+      <c r="C56" s="475" t="s">
         <v>160</v>
       </c>
-      <c r="D56" s="467"/>
-      <c r="E56" s="468"/>
+      <c r="D56" s="476"/>
+      <c r="E56" s="477"/>
     </row>
     <row r="57" spans="1:5" ht="15.95" customHeight="1">
       <c r="A57" s="28"/>
       <c r="B57" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="C57" s="466" t="s">
+      <c r="C57" s="475" t="s">
         <v>75</v>
       </c>
-      <c r="D57" s="467"/>
-      <c r="E57" s="468"/>
+      <c r="D57" s="476"/>
+      <c r="E57" s="477"/>
     </row>
     <row r="58" spans="1:5" ht="15.95" customHeight="1">
       <c r="A58" s="28"/>
       <c r="B58" s="46" t="s">
         <v>268</v>
       </c>
-      <c r="C58" s="466" t="s">
+      <c r="C58" s="475" t="s">
         <v>269</v>
       </c>
-      <c r="D58" s="467"/>
-      <c r="E58" s="468"/>
+      <c r="D58" s="476"/>
+      <c r="E58" s="477"/>
     </row>
     <row r="59" spans="1:5" ht="15.95" customHeight="1">
       <c r="A59" s="28"/>
       <c r="B59" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="C59" s="466" t="s">
+      <c r="C59" s="475" t="s">
         <v>77</v>
       </c>
-      <c r="D59" s="467"/>
-      <c r="E59" s="468"/>
+      <c r="D59" s="476"/>
+      <c r="E59" s="477"/>
     </row>
     <row r="60" spans="1:5" ht="15.95" customHeight="1">
       <c r="A60" s="28"/>
       <c r="B60" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="C60" s="466" t="s">
+      <c r="C60" s="475" t="s">
         <v>73</v>
       </c>
-      <c r="D60" s="467"/>
-      <c r="E60" s="468"/>
+      <c r="D60" s="476"/>
+      <c r="E60" s="477"/>
     </row>
     <row r="61" spans="1:5" ht="17.25" customHeight="1">
       <c r="A61" s="28"/>
       <c r="B61" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="C61" s="466" t="s">
+      <c r="C61" s="475" t="s">
         <v>79</v>
       </c>
-      <c r="D61" s="467"/>
-      <c r="E61" s="468"/>
+      <c r="D61" s="476"/>
+      <c r="E61" s="477"/>
     </row>
     <row r="62" spans="1:5" ht="27.75" customHeight="1">
       <c r="A62" s="28"/>
-      <c r="B62" s="474" t="s">
+      <c r="B62" s="468" t="s">
         <v>50</v>
       </c>
-      <c r="C62" s="475"/>
-      <c r="D62" s="475"/>
-      <c r="E62" s="476"/>
+      <c r="C62" s="469"/>
+      <c r="D62" s="469"/>
+      <c r="E62" s="470"/>
     </row>
     <row r="63" spans="1:5" ht="15.95" customHeight="1">
       <c r="A63" s="28"/>
       <c r="B63" s="46" t="s">
         <v>275</v>
       </c>
-      <c r="C63" s="477" t="s">
+      <c r="C63" s="471" t="s">
         <v>316</v>
       </c>
-      <c r="D63" s="478"/>
-      <c r="E63" s="479"/>
+      <c r="D63" s="472"/>
+      <c r="E63" s="473"/>
     </row>
     <row r="64" spans="1:5" ht="15.95" customHeight="1">
       <c r="A64" s="28"/>
       <c r="B64" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="C64" s="466" t="s">
+      <c r="C64" s="475" t="s">
         <v>317</v>
       </c>
-      <c r="D64" s="467"/>
-      <c r="E64" s="468"/>
+      <c r="D64" s="476"/>
+      <c r="E64" s="477"/>
     </row>
     <row r="65" spans="1:5" ht="39" customHeight="1">
       <c r="A65" s="28"/>
       <c r="B65" s="46" t="s">
         <v>134</v>
       </c>
-      <c r="C65" s="466" t="s">
+      <c r="C65" s="475" t="s">
         <v>318</v>
       </c>
-      <c r="D65" s="467"/>
-      <c r="E65" s="468"/>
+      <c r="D65" s="476"/>
+      <c r="E65" s="477"/>
     </row>
     <row r="66" spans="1:5" ht="28.5" customHeight="1">
       <c r="A66" s="28"/>
       <c r="B66" s="46" t="s">
         <v>126</v>
       </c>
-      <c r="C66" s="466" t="s">
+      <c r="C66" s="475" t="s">
         <v>86</v>
       </c>
-      <c r="D66" s="467"/>
-      <c r="E66" s="468"/>
+      <c r="D66" s="476"/>
+      <c r="E66" s="477"/>
     </row>
     <row r="67" spans="1:5" ht="15.75" customHeight="1">
       <c r="A67" s="28"/>
       <c r="B67" s="46" t="s">
         <v>138</v>
       </c>
-      <c r="C67" s="466" t="s">
+      <c r="C67" s="475" t="s">
         <v>83</v>
       </c>
-      <c r="D67" s="467"/>
-      <c r="E67" s="468"/>
+      <c r="D67" s="476"/>
+      <c r="E67" s="477"/>
     </row>
     <row r="68" spans="1:5" ht="15.75" customHeight="1">
       <c r="A68" s="28"/>
       <c r="B68" s="46" t="s">
         <v>137</v>
       </c>
-      <c r="C68" s="466" t="s">
+      <c r="C68" s="475" t="s">
         <v>80</v>
       </c>
-      <c r="D68" s="467"/>
-      <c r="E68" s="468"/>
+      <c r="D68" s="476"/>
+      <c r="E68" s="477"/>
     </row>
     <row r="69" spans="1:5" ht="15.75" customHeight="1">
       <c r="A69" s="28"/>
       <c r="B69" s="46" t="s">
         <v>126</v>
       </c>
-      <c r="C69" s="466" t="s">
+      <c r="C69" s="475" t="s">
         <v>86</v>
       </c>
-      <c r="D69" s="467"/>
-      <c r="E69" s="468"/>
+      <c r="D69" s="476"/>
+      <c r="E69" s="477"/>
     </row>
     <row r="70" spans="1:5" ht="15.75" customHeight="1">
       <c r="A70" s="28"/>
       <c r="B70" s="46" t="s">
         <v>139</v>
       </c>
-      <c r="C70" s="466" t="s">
+      <c r="C70" s="475" t="s">
         <v>84</v>
       </c>
-      <c r="D70" s="467"/>
-      <c r="E70" s="468"/>
+      <c r="D70" s="476"/>
+      <c r="E70" s="477"/>
     </row>
     <row r="71" spans="1:5" ht="15.75" customHeight="1">
       <c r="A71" s="28"/>
       <c r="B71" s="46" t="s">
         <v>137</v>
       </c>
-      <c r="C71" s="466" t="s">
+      <c r="C71" s="475" t="s">
         <v>81</v>
       </c>
-      <c r="D71" s="467"/>
-      <c r="E71" s="468"/>
+      <c r="D71" s="476"/>
+      <c r="E71" s="477"/>
     </row>
     <row r="72" spans="1:5" ht="15.75" customHeight="1">
       <c r="A72" s="28"/>
       <c r="B72" s="46" t="s">
         <v>126</v>
       </c>
-      <c r="C72" s="466" t="s">
+      <c r="C72" s="475" t="s">
         <v>86</v>
       </c>
-      <c r="D72" s="467"/>
-      <c r="E72" s="468"/>
+      <c r="D72" s="476"/>
+      <c r="E72" s="477"/>
     </row>
     <row r="73" spans="1:5" ht="15.75" customHeight="1">
       <c r="A73" s="28"/>
       <c r="B73" s="46" t="s">
         <v>140</v>
       </c>
-      <c r="C73" s="466" t="s">
+      <c r="C73" s="475" t="s">
         <v>85</v>
       </c>
-      <c r="D73" s="467"/>
-      <c r="E73" s="468"/>
+      <c r="D73" s="476"/>
+      <c r="E73" s="477"/>
     </row>
     <row r="74" spans="1:5" ht="15.75" customHeight="1">
       <c r="A74" s="28"/>
       <c r="B74" s="46" t="s">
         <v>137</v>
       </c>
-      <c r="C74" s="466" t="s">
+      <c r="C74" s="475" t="s">
         <v>82</v>
       </c>
-      <c r="D74" s="467"/>
-      <c r="E74" s="468"/>
+      <c r="D74" s="476"/>
+      <c r="E74" s="477"/>
     </row>
     <row r="75" spans="1:5" ht="15.75" customHeight="1">
       <c r="A75" s="28"/>
@@ -12800,23 +12950,23 @@
       <c r="E78" s="373"/>
     </row>
     <row r="79" spans="1:5" s="16" customFormat="1" ht="16.5" customHeight="1">
-      <c r="B79" s="469"/>
-      <c r="C79" s="469"/>
-      <c r="D79" s="469"/>
-      <c r="E79" s="469"/>
+      <c r="B79" s="463"/>
+      <c r="C79" s="463"/>
+      <c r="D79" s="463"/>
+      <c r="E79" s="463"/>
     </row>
     <row r="80" spans="1:5" s="16" customFormat="1" ht="13.5" customHeight="1">
       <c r="B80" s="361"/>
-      <c r="C80" s="470"/>
-      <c r="D80" s="470"/>
-      <c r="E80" s="470"/>
+      <c r="C80" s="464"/>
+      <c r="D80" s="464"/>
+      <c r="E80" s="464"/>
     </row>
     <row r="81" spans="1:5" ht="15.95" customHeight="1">
       <c r="A81" s="28"/>
-      <c r="B81" s="480"/>
-      <c r="C81" s="480"/>
-      <c r="D81" s="480"/>
-      <c r="E81" s="480"/>
+      <c r="B81" s="474"/>
+      <c r="C81" s="474"/>
+      <c r="D81" s="474"/>
+      <c r="E81" s="474"/>
     </row>
     <row r="82" spans="1:5" ht="15.95" customHeight="1">
       <c r="A82" s="28"/>
@@ -12876,10 +13026,10 @@
     </row>
     <row r="90" spans="1:5" ht="15.95" customHeight="1">
       <c r="A90" s="28"/>
-      <c r="B90" s="480"/>
-      <c r="C90" s="480"/>
-      <c r="D90" s="480"/>
-      <c r="E90" s="480"/>
+      <c r="B90" s="474"/>
+      <c r="C90" s="474"/>
+      <c r="D90" s="474"/>
+      <c r="E90" s="474"/>
     </row>
     <row r="91" spans="1:5" ht="15.95" customHeight="1">
       <c r="A91" s="28"/>
@@ -12990,26 +13140,26 @@
     </row>
     <row r="106" spans="1:6">
       <c r="A106" s="29"/>
-      <c r="B106" s="469"/>
-      <c r="C106" s="469"/>
-      <c r="D106" s="469"/>
-      <c r="E106" s="469"/>
+      <c r="B106" s="463"/>
+      <c r="C106" s="463"/>
+      <c r="D106" s="463"/>
+      <c r="E106" s="463"/>
       <c r="F106" s="36"/>
     </row>
     <row r="107" spans="1:6">
       <c r="A107" s="29"/>
       <c r="B107" s="361"/>
-      <c r="C107" s="470"/>
-      <c r="D107" s="470"/>
-      <c r="E107" s="470"/>
+      <c r="C107" s="464"/>
+      <c r="D107" s="464"/>
+      <c r="E107" s="464"/>
       <c r="F107" s="36"/>
     </row>
     <row r="108" spans="1:6">
       <c r="A108" s="29"/>
-      <c r="B108" s="480"/>
-      <c r="C108" s="480"/>
-      <c r="D108" s="480"/>
-      <c r="E108" s="480"/>
+      <c r="B108" s="474"/>
+      <c r="C108" s="474"/>
+      <c r="D108" s="474"/>
+      <c r="E108" s="474"/>
       <c r="F108" s="36"/>
     </row>
     <row r="109" spans="1:6" ht="12.75" customHeight="1">
@@ -13078,10 +13228,10 @@
     </row>
     <row r="117" spans="1:6">
       <c r="A117" s="29"/>
-      <c r="B117" s="480"/>
-      <c r="C117" s="480"/>
-      <c r="D117" s="480"/>
-      <c r="E117" s="480"/>
+      <c r="B117" s="474"/>
+      <c r="C117" s="474"/>
+      <c r="D117" s="474"/>
+      <c r="E117" s="474"/>
       <c r="F117" s="36"/>
     </row>
     <row r="118" spans="1:6">
@@ -13206,26 +13356,26 @@
     </row>
     <row r="133" spans="1:6" ht="12.75" customHeight="1">
       <c r="A133" s="29"/>
-      <c r="B133" s="469"/>
-      <c r="C133" s="469"/>
-      <c r="D133" s="469"/>
-      <c r="E133" s="469"/>
+      <c r="B133" s="463"/>
+      <c r="C133" s="463"/>
+      <c r="D133" s="463"/>
+      <c r="E133" s="463"/>
       <c r="F133" s="36"/>
     </row>
     <row r="134" spans="1:6">
       <c r="A134" s="29"/>
       <c r="B134" s="361"/>
-      <c r="C134" s="470"/>
-      <c r="D134" s="470"/>
-      <c r="E134" s="470"/>
+      <c r="C134" s="464"/>
+      <c r="D134" s="464"/>
+      <c r="E134" s="464"/>
       <c r="F134" s="36"/>
     </row>
     <row r="135" spans="1:6">
       <c r="A135" s="29"/>
-      <c r="B135" s="480"/>
-      <c r="C135" s="480"/>
-      <c r="D135" s="480"/>
-      <c r="E135" s="480"/>
+      <c r="B135" s="474"/>
+      <c r="C135" s="474"/>
+      <c r="D135" s="474"/>
+      <c r="E135" s="474"/>
       <c r="F135" s="36"/>
     </row>
     <row r="136" spans="1:6" ht="12.75" customHeight="1">
@@ -13294,10 +13444,10 @@
     </row>
     <row r="144" spans="1:6">
       <c r="A144" s="29"/>
-      <c r="B144" s="480"/>
-      <c r="C144" s="480"/>
-      <c r="D144" s="480"/>
-      <c r="E144" s="480"/>
+      <c r="B144" s="474"/>
+      <c r="C144" s="474"/>
+      <c r="D144" s="474"/>
+      <c r="E144" s="474"/>
       <c r="F144" s="36"/>
     </row>
     <row r="145" spans="1:6">
@@ -13422,26 +13572,26 @@
     </row>
     <row r="160" spans="1:6">
       <c r="A160" s="29"/>
-      <c r="B160" s="469"/>
-      <c r="C160" s="469"/>
-      <c r="D160" s="469"/>
-      <c r="E160" s="469"/>
+      <c r="B160" s="463"/>
+      <c r="C160" s="463"/>
+      <c r="D160" s="463"/>
+      <c r="E160" s="463"/>
       <c r="F160" s="36"/>
     </row>
     <row r="161" spans="1:6">
       <c r="A161" s="29"/>
       <c r="B161" s="361"/>
-      <c r="C161" s="470"/>
-      <c r="D161" s="470"/>
-      <c r="E161" s="470"/>
+      <c r="C161" s="464"/>
+      <c r="D161" s="464"/>
+      <c r="E161" s="464"/>
       <c r="F161" s="36"/>
     </row>
     <row r="162" spans="1:6">
       <c r="A162" s="29"/>
-      <c r="B162" s="480"/>
-      <c r="C162" s="480"/>
-      <c r="D162" s="480"/>
-      <c r="E162" s="480"/>
+      <c r="B162" s="474"/>
+      <c r="C162" s="474"/>
+      <c r="D162" s="474"/>
+      <c r="E162" s="474"/>
       <c r="F162" s="36"/>
     </row>
     <row r="163" spans="1:6" ht="12.75" customHeight="1">
@@ -13510,10 +13660,10 @@
     </row>
     <row r="171" spans="1:6">
       <c r="A171" s="29"/>
-      <c r="B171" s="480"/>
-      <c r="C171" s="480"/>
-      <c r="D171" s="480"/>
-      <c r="E171" s="480"/>
+      <c r="B171" s="474"/>
+      <c r="C171" s="474"/>
+      <c r="D171" s="474"/>
+      <c r="E171" s="474"/>
       <c r="F171" s="36"/>
     </row>
     <row r="172" spans="1:6">
@@ -13638,26 +13788,26 @@
     </row>
     <row r="187" spans="1:6">
       <c r="A187" s="29"/>
-      <c r="B187" s="469"/>
-      <c r="C187" s="469"/>
-      <c r="D187" s="469"/>
-      <c r="E187" s="469"/>
+      <c r="B187" s="463"/>
+      <c r="C187" s="463"/>
+      <c r="D187" s="463"/>
+      <c r="E187" s="463"/>
       <c r="F187" s="36"/>
     </row>
     <row r="188" spans="1:6">
       <c r="A188" s="29"/>
       <c r="B188" s="361"/>
-      <c r="C188" s="470"/>
-      <c r="D188" s="470"/>
-      <c r="E188" s="470"/>
+      <c r="C188" s="464"/>
+      <c r="D188" s="464"/>
+      <c r="E188" s="464"/>
       <c r="F188" s="36"/>
     </row>
     <row r="189" spans="1:6">
       <c r="A189" s="29"/>
-      <c r="B189" s="480"/>
-      <c r="C189" s="480"/>
-      <c r="D189" s="480"/>
-      <c r="E189" s="480"/>
+      <c r="B189" s="474"/>
+      <c r="C189" s="474"/>
+      <c r="D189" s="474"/>
+      <c r="E189" s="474"/>
       <c r="F189" s="36"/>
     </row>
     <row r="190" spans="1:6" ht="12.75" customHeight="1">
@@ -13726,10 +13876,10 @@
     </row>
     <row r="198" spans="1:6">
       <c r="A198" s="29"/>
-      <c r="B198" s="480"/>
-      <c r="C198" s="480"/>
-      <c r="D198" s="480"/>
-      <c r="E198" s="480"/>
+      <c r="B198" s="474"/>
+      <c r="C198" s="474"/>
+      <c r="D198" s="474"/>
+      <c r="E198" s="474"/>
       <c r="F198" s="36"/>
     </row>
     <row r="199" spans="1:6">
@@ -13854,26 +14004,26 @@
     </row>
     <row r="214" spans="1:9">
       <c r="A214" s="29"/>
-      <c r="B214" s="469"/>
-      <c r="C214" s="469"/>
-      <c r="D214" s="469"/>
-      <c r="E214" s="469"/>
+      <c r="B214" s="463"/>
+      <c r="C214" s="463"/>
+      <c r="D214" s="463"/>
+      <c r="E214" s="463"/>
       <c r="F214" s="36"/>
     </row>
     <row r="215" spans="1:9" ht="12.75" customHeight="1">
       <c r="A215" s="28"/>
       <c r="B215" s="361"/>
-      <c r="C215" s="470"/>
-      <c r="D215" s="470"/>
-      <c r="E215" s="470"/>
+      <c r="C215" s="464"/>
+      <c r="D215" s="464"/>
+      <c r="E215" s="464"/>
       <c r="F215" s="36"/>
     </row>
     <row r="216" spans="1:9" ht="12.75" customHeight="1">
       <c r="A216" s="29"/>
       <c r="B216" s="362"/>
-      <c r="C216" s="471"/>
-      <c r="D216" s="471"/>
-      <c r="E216" s="471"/>
+      <c r="C216" s="465"/>
+      <c r="D216" s="465"/>
+      <c r="E216" s="465"/>
       <c r="F216" s="128"/>
       <c r="G216" s="128"/>
       <c r="H216" s="128"/>
@@ -13882,18 +14032,18 @@
     <row r="217" spans="1:9" ht="12.75" customHeight="1">
       <c r="A217" s="29"/>
       <c r="B217" s="362"/>
-      <c r="C217" s="471"/>
-      <c r="D217" s="471"/>
-      <c r="E217" s="471"/>
+      <c r="C217" s="465"/>
+      <c r="D217" s="465"/>
+      <c r="E217" s="465"/>
       <c r="H217" s="128"/>
       <c r="I217" s="128"/>
     </row>
     <row r="218" spans="1:9">
       <c r="A218" s="29"/>
       <c r="B218" s="363"/>
-      <c r="C218" s="471"/>
-      <c r="D218" s="471"/>
-      <c r="E218" s="471"/>
+      <c r="C218" s="465"/>
+      <c r="D218" s="465"/>
+      <c r="E218" s="465"/>
       <c r="H218" s="128"/>
       <c r="I218" s="128"/>
     </row>
@@ -13926,9 +14076,9 @@
     <row r="222" spans="1:9" ht="12.75" customHeight="1">
       <c r="A222" s="29"/>
       <c r="B222" s="461"/>
-      <c r="C222" s="473"/>
-      <c r="D222" s="473"/>
-      <c r="E222" s="473"/>
+      <c r="C222" s="467"/>
+      <c r="D222" s="467"/>
+      <c r="E222" s="467"/>
       <c r="F222" s="308"/>
     </row>
     <row r="223" spans="1:9" ht="12.75" customHeight="1">
@@ -13943,7 +14093,7 @@
       <c r="A224" s="29"/>
       <c r="B224" s="367"/>
       <c r="C224" s="367"/>
-      <c r="D224" s="472"/>
+      <c r="D224" s="466"/>
       <c r="E224" s="309"/>
       <c r="F224" s="309"/>
     </row>
@@ -13951,7 +14101,7 @@
       <c r="A225" s="29"/>
       <c r="B225" s="309"/>
       <c r="C225" s="309"/>
-      <c r="D225" s="472"/>
+      <c r="D225" s="466"/>
       <c r="E225" s="309"/>
       <c r="F225" s="309"/>
     </row>
@@ -15065,9 +15215,6 @@
     <mergeCell ref="C47:E47"/>
     <mergeCell ref="C74:E74"/>
     <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C86:E86"/>
-    <mergeCell ref="C88:E88"/>
-    <mergeCell ref="C89:E89"/>
     <mergeCell ref="C68:E68"/>
     <mergeCell ref="C92:E92"/>
     <mergeCell ref="B79:E79"/>
@@ -15151,6 +15298,9 @@
     <mergeCell ref="B135:E135"/>
     <mergeCell ref="C136:E136"/>
     <mergeCell ref="C137:E137"/>
+    <mergeCell ref="C86:E86"/>
+    <mergeCell ref="C88:E88"/>
+    <mergeCell ref="C89:E89"/>
     <mergeCell ref="B241:C241"/>
     <mergeCell ref="B249:C249"/>
     <mergeCell ref="C219:E219"/>
@@ -42148,12 +42298,6 @@
     </row>
   </sheetData>
   <mergeCells count="253">
-    <mergeCell ref="M52:N52"/>
-    <mergeCell ref="M55:N55"/>
-    <mergeCell ref="M54:N54"/>
-    <mergeCell ref="M66:N66"/>
-    <mergeCell ref="M68:N68"/>
-    <mergeCell ref="M70:N70"/>
     <mergeCell ref="M249:N249"/>
     <mergeCell ref="M239:N239"/>
     <mergeCell ref="M240:N240"/>
@@ -42164,9 +42308,16 @@
     <mergeCell ref="M246:N246"/>
     <mergeCell ref="M247:N247"/>
     <mergeCell ref="M248:N248"/>
-    <mergeCell ref="A1:N5"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="F17:N17"/>
+    <mergeCell ref="M169:N169"/>
+    <mergeCell ref="M170:N170"/>
+    <mergeCell ref="M176:N176"/>
+    <mergeCell ref="M178:N178"/>
+    <mergeCell ref="B172:E172"/>
+    <mergeCell ref="M177:N177"/>
+    <mergeCell ref="B171:E171"/>
+    <mergeCell ref="M146:N146"/>
+    <mergeCell ref="M154:N154"/>
+    <mergeCell ref="M155:N155"/>
     <mergeCell ref="M227:N227"/>
     <mergeCell ref="M228:N228"/>
     <mergeCell ref="M229:N229"/>
@@ -42178,27 +42329,6 @@
     <mergeCell ref="M210:N210"/>
     <mergeCell ref="M211:N211"/>
     <mergeCell ref="M212:N212"/>
-    <mergeCell ref="M169:N169"/>
-    <mergeCell ref="M170:N170"/>
-    <mergeCell ref="M176:N176"/>
-    <mergeCell ref="M178:N178"/>
-    <mergeCell ref="B172:E172"/>
-    <mergeCell ref="M177:N177"/>
-    <mergeCell ref="B171:E171"/>
-    <mergeCell ref="M146:N146"/>
-    <mergeCell ref="M154:N154"/>
-    <mergeCell ref="M155:N155"/>
-    <mergeCell ref="M122:N122"/>
-    <mergeCell ref="M123:N123"/>
-    <mergeCell ref="M124:N124"/>
-    <mergeCell ref="B153:E153"/>
-    <mergeCell ref="B159:E159"/>
-    <mergeCell ref="B165:E165"/>
-    <mergeCell ref="M160:N160"/>
-    <mergeCell ref="M161:N161"/>
-    <mergeCell ref="M162:N162"/>
-    <mergeCell ref="M163:N163"/>
-    <mergeCell ref="M158:N158"/>
     <mergeCell ref="M141:N141"/>
     <mergeCell ref="M142:N142"/>
     <mergeCell ref="M143:N143"/>
@@ -42206,6 +42336,18 @@
     <mergeCell ref="M145:N145"/>
     <mergeCell ref="M156:N156"/>
     <mergeCell ref="M157:N157"/>
+    <mergeCell ref="A1:N5"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="F17:N17"/>
+    <mergeCell ref="M52:N52"/>
+    <mergeCell ref="M55:N55"/>
+    <mergeCell ref="M54:N54"/>
+    <mergeCell ref="M66:N66"/>
+    <mergeCell ref="M68:N68"/>
+    <mergeCell ref="M70:N70"/>
+    <mergeCell ref="M122:N122"/>
+    <mergeCell ref="M123:N123"/>
+    <mergeCell ref="M124:N124"/>
     <mergeCell ref="M128:N128"/>
     <mergeCell ref="M129:N129"/>
     <mergeCell ref="M130:N130"/>
@@ -42337,6 +42479,14 @@
     <mergeCell ref="M166:N166"/>
     <mergeCell ref="M167:N167"/>
     <mergeCell ref="M168:N168"/>
+    <mergeCell ref="B153:E153"/>
+    <mergeCell ref="B159:E159"/>
+    <mergeCell ref="B165:E165"/>
+    <mergeCell ref="M160:N160"/>
+    <mergeCell ref="M161:N161"/>
+    <mergeCell ref="M162:N162"/>
+    <mergeCell ref="M163:N163"/>
+    <mergeCell ref="M158:N158"/>
     <mergeCell ref="M186:N186"/>
     <mergeCell ref="M180:N180"/>
     <mergeCell ref="M181:N181"/>
@@ -42456,8 +42606,8 @@
   </sheetPr>
   <dimension ref="A1:AO279"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A239" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O145" sqref="O145"/>
+    <sheetView tabSelected="1" topLeftCell="A223" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B227" sqref="B227:E227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -45088,7 +45238,7 @@
     </row>
     <row r="48" spans="1:41" ht="60" customHeight="1">
       <c r="B48" s="569" t="s">
-        <v>305</v>
+        <v>472</v>
       </c>
       <c r="C48" s="569"/>
       <c r="D48" s="569"/>
@@ -45454,7 +45604,7 @@
     </row>
     <row r="54" spans="1:41" ht="60" customHeight="1">
       <c r="B54" s="569" t="s">
-        <v>304</v>
+        <v>473</v>
       </c>
       <c r="C54" s="569"/>
       <c r="D54" s="569"/>
@@ -47311,7 +47461,7 @@
     </row>
     <row r="85" spans="1:41" ht="60" customHeight="1">
       <c r="B85" s="569" t="s">
-        <v>303</v>
+        <v>471</v>
       </c>
       <c r="C85" s="569"/>
       <c r="D85" s="569"/>
@@ -49141,7 +49291,7 @@
     </row>
     <row r="115" spans="1:41" ht="60" customHeight="1">
       <c r="B115" s="569" t="s">
-        <v>430</v>
+        <v>470</v>
       </c>
       <c r="C115" s="569"/>
       <c r="D115" s="569"/>
@@ -49507,7 +49657,7 @@
     </row>
     <row r="121" spans="1:41" ht="60" customHeight="1">
       <c r="B121" s="569" t="s">
-        <v>431</v>
+        <v>469</v>
       </c>
       <c r="C121" s="569"/>
       <c r="D121" s="569"/>
@@ -51364,7 +51514,7 @@
     </row>
     <row r="152" spans="1:41" ht="60" customHeight="1">
       <c r="B152" s="570" t="s">
-        <v>306</v>
+        <v>474</v>
       </c>
       <c r="C152" s="595"/>
       <c r="D152" s="595"/>
@@ -55838,7 +55988,7 @@
     </row>
     <row r="227" spans="1:41" ht="60" customHeight="1">
       <c r="B227" s="575" t="s">
-        <v>451</v>
+        <v>478</v>
       </c>
       <c r="C227" s="575"/>
       <c r="D227" s="575"/>
@@ -56204,7 +56354,7 @@
     </row>
     <row r="233" spans="1:41" ht="60" customHeight="1">
       <c r="B233" s="569" t="s">
-        <v>452</v>
+        <v>477</v>
       </c>
       <c r="C233" s="569"/>
       <c r="D233" s="569"/>
@@ -56570,7 +56720,7 @@
     </row>
     <row r="239" spans="1:41" ht="60" customHeight="1">
       <c r="B239" s="569" t="s">
-        <v>453</v>
+        <v>476</v>
       </c>
       <c r="C239" s="569"/>
       <c r="D239" s="569"/>
@@ -56936,7 +57086,7 @@
     </row>
     <row r="245" spans="1:41" ht="60" customHeight="1">
       <c r="B245" s="569" t="s">
-        <v>308</v>
+        <v>475</v>
       </c>
       <c r="C245" s="569"/>
       <c r="D245" s="569"/>

</xml_diff>